<commit_message>
DDT Robot Excel File Modified
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -31,13 +31,10 @@
     <t xml:space="preserve">${password}</t>
   </si>
   <si>
-    <t xml:space="preserve">${error_msg}</t>
+    <t xml:space="preserve">${expected_error_msg}</t>
   </si>
   <si>
     <t xml:space="preserve">Empty User Name and Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“”</t>
   </si>
   <si>
     <t xml:space="preserve">Epic sadface: Username is required</t>
@@ -173,15 +170,15 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -203,84 +200,72 @@
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>